<commit_message>
Fixed Column Selector and File Download
The column selector now works and opens up the modal after upload.

The issue with the download  was that write-excel-file has to have "schema" and not another variable with the word schema
</commit_message>
<xml_diff>
--- a/Test Files/raffle-test-data.xlsx
+++ b/Test Files/raffle-test-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/familycomp/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vom3-2/Documents/Coding Projects/JS/excel-scroll-winner/Test Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{529D0753-6103-BA42-BB47-922C34D42CE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DBE5B97-DD09-2646-B17B-3E2605ACB38B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5460" windowWidth="28040" windowHeight="17440" xr2:uid="{BBD95963-BAAC-0440-A6EA-9A9A4CC60039}"/>
+    <workbookView xWindow="6580" yWindow="1360" windowWidth="28040" windowHeight="17440" xr2:uid="{BBD95963-BAAC-0440-A6EA-9A9A4CC60039}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="108">
   <si>
     <t>Ben</t>
   </si>
@@ -186,13 +186,187 @@
   </si>
   <si>
     <t>Brenner</t>
+  </si>
+  <si>
+    <t>Last</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Ticket</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>740-404-0975</t>
+  </si>
+  <si>
+    <t>740-404-0976</t>
+  </si>
+  <si>
+    <t>740-404-0977</t>
+  </si>
+  <si>
+    <t>740-404-0978</t>
+  </si>
+  <si>
+    <t>740-404-0979</t>
+  </si>
+  <si>
+    <t>740-404-0980</t>
+  </si>
+  <si>
+    <t>740-404-0981</t>
+  </si>
+  <si>
+    <t>740-404-0982</t>
+  </si>
+  <si>
+    <t>740-404-0983</t>
+  </si>
+  <si>
+    <t>740-404-0984</t>
+  </si>
+  <si>
+    <t>740-404-0985</t>
+  </si>
+  <si>
+    <t>740-404-0986</t>
+  </si>
+  <si>
+    <t>740-404-0987</t>
+  </si>
+  <si>
+    <t>740-404-0988</t>
+  </si>
+  <si>
+    <t>740-404-0989</t>
+  </si>
+  <si>
+    <t>740-404-0990</t>
+  </si>
+  <si>
+    <t>740-404-0991</t>
+  </si>
+  <si>
+    <t>740-404-0992</t>
+  </si>
+  <si>
+    <t>740-404-0993</t>
+  </si>
+  <si>
+    <t>740-404-0994</t>
+  </si>
+  <si>
+    <t>740-404-0995</t>
+  </si>
+  <si>
+    <t>740-404-0996</t>
+  </si>
+  <si>
+    <t>740-404-0997</t>
+  </si>
+  <si>
+    <t>740-404-0998</t>
+  </si>
+  <si>
+    <t>740-404-0999</t>
+  </si>
+  <si>
+    <t>740-404-1000</t>
+  </si>
+  <si>
+    <t>740-404-1001</t>
+  </si>
+  <si>
+    <t>740-404-1002</t>
+  </si>
+  <si>
+    <t>740-404-1003</t>
+  </si>
+  <si>
+    <t>740-404-1004</t>
+  </si>
+  <si>
+    <t>740-404-1005</t>
+  </si>
+  <si>
+    <t>740-404-1006</t>
+  </si>
+  <si>
+    <t>740-404-1007</t>
+  </si>
+  <si>
+    <t>740-404-1008</t>
+  </si>
+  <si>
+    <t>740-404-1009</t>
+  </si>
+  <si>
+    <t>740-404-1010</t>
+  </si>
+  <si>
+    <t>740-404-1011</t>
+  </si>
+  <si>
+    <t>740-404-1012</t>
+  </si>
+  <si>
+    <t>740-404-1013</t>
+  </si>
+  <si>
+    <t>740-404-1014</t>
+  </si>
+  <si>
+    <t>740-404-1015</t>
+  </si>
+  <si>
+    <t>740-404-1016</t>
+  </si>
+  <si>
+    <t>740-404-1017</t>
+  </si>
+  <si>
+    <t>740-404-1018</t>
+  </si>
+  <si>
+    <t>740-404-1019</t>
+  </si>
+  <si>
+    <t>740-404-1020</t>
+  </si>
+  <si>
+    <t>740-404-1021</t>
+  </si>
+  <si>
+    <t>740-404-1022</t>
+  </si>
+  <si>
+    <t>740-404-1023</t>
+  </si>
+  <si>
+    <t>740-404-1024</t>
+  </si>
+  <si>
+    <t>740-404-1025</t>
+  </si>
+  <si>
+    <t>740-404-1026</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[&lt;=9999999]###\-####;\(###\)\ ###\-####"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -204,6 +378,12 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -230,9 +410,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -252,9 +433,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -292,7 +473,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -398,7 +579,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -540,7 +721,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -548,645 +729,976 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F50870C8-3048-064B-8E58-D6EAEBB03DE3}">
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C52"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="1" t="str">
-        <f>CONCATENATE(A1,".",B1,"@","exmaple.com")</f>
+      <c r="C2" s="1" t="str">
+        <f>CONCATENATE(A2,".",B2,"@","exmaple.com")</f>
         <v>Ben.Smith@exmaple.com</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="D2">
+        <v>23836</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="1" t="str">
-        <f t="shared" ref="C2:C52" si="0">CONCATENATE(A2,".",B2,"@","exmaple.com")</f>
+      <c r="C3" s="1" t="str">
+        <f t="shared" ref="C3:C53" si="0">CONCATENATE(A3,".",B3,"@","exmaple.com")</f>
         <v>Don.Johnson@exmaple.com</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="D3">
+        <v>23836</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="1" t="str">
+      <c r="C4" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Alice.LaCroix@exmaple.com</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="D4">
+        <v>23836</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="1" t="str">
+      <c r="C5" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Jimmy.Hoffe@exmaple.com</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="D5">
+        <v>23836</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="1" t="str">
+      <c r="C6" s="1" t="str">
         <f t="shared" si="0"/>
         <v>dan.De'Vito@exmaple.com</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="D6">
+        <v>23836</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="1" t="str">
+      <c r="C7" s="1" t="str">
         <f t="shared" si="0"/>
         <v>mark.Hamil@exmaple.com</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="D7">
+        <v>23836</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="1" t="str">
+      <c r="C8" s="1" t="str">
         <f t="shared" si="0"/>
         <v>shawn.Watson@exmaple.com</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="D8">
+        <v>23836</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="1" t="str">
+      <c r="C9" s="1" t="str">
         <f t="shared" si="0"/>
         <v>evan.Swanson@exmaple.com</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="D9">
+        <v>23836</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="1" t="str">
+      <c r="C10" s="1" t="str">
         <f t="shared" si="0"/>
         <v>hannah.Montana@exmaple.com</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="D10">
+        <v>23836</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="1" t="str">
+      <c r="C11" s="1" t="str">
         <f t="shared" si="0"/>
         <v>charlotte.Duchess@exmaple.com</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="D11">
+        <v>23836</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="1" t="str">
+      <c r="C12" s="1" t="str">
         <f t="shared" si="0"/>
         <v>lindsey.Lohan@exmaple.com</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="D12">
+        <v>23836</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="1" t="str">
+      <c r="C13" s="1" t="str">
         <f t="shared" si="0"/>
         <v>savannah.Bananas@exmaple.com</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="D13">
+        <v>23836</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="1" t="str">
+      <c r="C14" s="1" t="str">
         <f t="shared" si="0"/>
         <v>emily.Blunt@exmaple.com</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="D14">
+        <v>23836</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="1" t="str">
+      <c r="C15" s="1" t="str">
         <f t="shared" si="0"/>
         <v>alise.Sheran@exmaple.com</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="D15">
+        <v>23836</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="1" t="str">
+      <c r="C16" s="1" t="str">
         <f t="shared" si="0"/>
         <v>lisa.Ludrow@exmaple.com</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="D16">
+        <v>23836</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="1" t="str">
+      <c r="C17" s="1" t="str">
         <f t="shared" si="0"/>
         <v>kyle.Walker@exmaple.com</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="D17">
+        <v>23836</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="1" t="str">
+      <c r="C18" s="1" t="str">
         <f t="shared" si="0"/>
         <v>jordan.Michael@exmaple.com</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="D18">
+        <v>23836</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>42</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="1" t="str">
+      <c r="C19" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Sam.Smith@exmaple.com</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="D19">
+        <v>23836</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="1" t="str">
+      <c r="C20" s="1" t="str">
         <f t="shared" si="0"/>
         <v>david.Goliath@exmaple.com</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="D20">
+        <v>23836</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>44</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="1" t="str">
+      <c r="C21" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Nate.Bonaparte@exmaple.com</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="D21">
+        <v>23836</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="1" t="str">
+      <c r="C22" s="1" t="str">
         <f t="shared" si="0"/>
         <v>tom.Holland@exmaple.com</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="D22">
+        <v>23836</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="1" t="str">
+      <c r="C23" s="1" t="str">
         <f t="shared" si="0"/>
         <v>duke.Nukem@exmaple.com</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="D23">
+        <v>23836</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="1" t="str">
+      <c r="C24" s="1" t="str">
         <f t="shared" si="0"/>
         <v>kim.Kardashian@exmaple.com</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="D24">
+        <v>23836</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="1" t="str">
+      <c r="C25" s="1" t="str">
         <f t="shared" si="0"/>
         <v>kylie.Jenner@exmaple.com</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="D25">
+        <v>23836</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="1" t="str">
+      <c r="C26" s="1" t="str">
         <f t="shared" si="0"/>
         <v>corry.Brenner@exmaple.com</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="D26">
+        <v>23836</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>0</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="1" t="str">
+      <c r="C27" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Ben.Smith@exmaple.com</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="D27">
+        <v>23836</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>1</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="1" t="str">
+      <c r="C28" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Don.Johnson@exmaple.com</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="D28">
+        <v>23836</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>2</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="1" t="str">
+      <c r="C29" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Alice.LaCroix@exmaple.com</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="D29">
+        <v>23836</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>3</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="1" t="str">
+      <c r="C30" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Jimmy.Hoffe@exmaple.com</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="D30">
+        <v>23836</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>4</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="1" t="str">
+      <c r="C31" s="1" t="str">
         <f t="shared" si="0"/>
         <v>dan.De'Vito@exmaple.com</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="D31">
+        <v>23836</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>5</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="1" t="str">
+      <c r="C32" s="1" t="str">
         <f t="shared" si="0"/>
         <v>mark.Hamil@exmaple.com</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="D32">
+        <v>23836</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>6</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="1" t="str">
+      <c r="C33" s="1" t="str">
         <f t="shared" si="0"/>
         <v>shawn.Watson@exmaple.com</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="D33">
+        <v>23836</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>7</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="1" t="str">
+      <c r="C34" s="1" t="str">
         <f t="shared" si="0"/>
         <v>evan.Swanson@exmaple.com</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="D34">
+        <v>23836</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>8</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="1" t="str">
+      <c r="C35" s="1" t="str">
         <f t="shared" si="0"/>
         <v>hannah.Montana@exmaple.com</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="D35">
+        <v>23836</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>9</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="1" t="str">
+      <c r="C36" s="1" t="str">
         <f t="shared" si="0"/>
         <v>charlotte.Duchess@exmaple.com</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="D36">
+        <v>23836</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>10</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>35</v>
       </c>
-      <c r="C36" s="1" t="str">
+      <c r="C37" s="1" t="str">
         <f t="shared" si="0"/>
         <v>lindsey.Lohan@exmaple.com</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="D37">
+        <v>23836</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>11</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="1" t="str">
+      <c r="C38" s="1" t="str">
         <f t="shared" si="0"/>
         <v>savannah.Bananas@exmaple.com</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="D38">
+        <v>23836</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>12</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>37</v>
       </c>
-      <c r="C38" s="1" t="str">
+      <c r="C39" s="1" t="str">
         <f t="shared" si="0"/>
         <v>emily.Blunt@exmaple.com</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="D39">
+        <v>23836</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>13</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="1" t="str">
+      <c r="C40" s="1" t="str">
         <f t="shared" si="0"/>
         <v>alise.Sheran@exmaple.com</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="D40">
+        <v>23836</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>14</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>39</v>
       </c>
-      <c r="C40" s="1" t="str">
+      <c r="C41" s="1" t="str">
         <f t="shared" si="0"/>
         <v>lisa.Ludrow@exmaple.com</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="D41">
+        <v>23836</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>15</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="1" t="str">
+      <c r="C42" s="1" t="str">
         <f t="shared" si="0"/>
         <v>kyle.Walker@exmaple.com</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="D42">
+        <v>23836</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>16</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>41</v>
       </c>
-      <c r="C42" s="1" t="str">
+      <c r="C43" s="1" t="str">
         <f t="shared" si="0"/>
         <v>jordan.Michael@exmaple.com</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="D43">
+        <v>23836</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>17</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>25</v>
       </c>
-      <c r="C43" s="1" t="str">
+      <c r="C44" s="1" t="str">
         <f t="shared" si="0"/>
         <v>sma.Smith@exmaple.com</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="D44">
+        <v>23836</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>18</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>43</v>
       </c>
-      <c r="C44" s="1" t="str">
+      <c r="C45" s="1" t="str">
         <f t="shared" si="0"/>
         <v>david.Goliath@exmaple.com</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="D45">
+        <v>23836</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>19</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>45</v>
       </c>
-      <c r="C45" s="1" t="str">
+      <c r="C46" s="1" t="str">
         <f t="shared" si="0"/>
         <v>nat.Bonaparte@exmaple.com</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="D46">
+        <v>23836</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>20</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>46</v>
       </c>
-      <c r="C46" s="1" t="str">
+      <c r="C47" s="1" t="str">
         <f t="shared" si="0"/>
         <v>tom.Holland@exmaple.com</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="D47">
+        <v>23836</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>21</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>47</v>
       </c>
-      <c r="C47" s="1" t="str">
+      <c r="C48" s="1" t="str">
         <f t="shared" si="0"/>
         <v>duke.Nukem@exmaple.com</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+      <c r="D48">
+        <v>23836</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>22</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>48</v>
       </c>
-      <c r="C48" s="1" t="str">
+      <c r="C49" s="1" t="str">
         <f t="shared" si="0"/>
         <v>kim.Kardashian@exmaple.com</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="D49">
+        <v>23836</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>23</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>49</v>
       </c>
-      <c r="C49" s="1" t="str">
+      <c r="C50" s="1" t="str">
         <f t="shared" si="0"/>
         <v>kylie.Jenner@exmaple.com</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="D50">
+        <v>23836</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>24</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>50</v>
       </c>
-      <c r="C50" s="1" t="str">
+      <c r="C51" s="1" t="str">
         <f t="shared" si="0"/>
         <v>corry.Brenner@exmaple.com</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+      <c r="D51">
+        <v>23836</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>0</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>25</v>
       </c>
-      <c r="C51" s="1" t="str">
+      <c r="C52" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Ben.Smith@exmaple.com</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+      <c r="D52">
+        <v>23836</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>1</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>26</v>
       </c>
-      <c r="C52" s="1" t="str">
+      <c r="C53" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Don.Johnson@exmaple.com</v>
       </c>
+      <c r="D53">
+        <v>23836</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>107</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1" display="b.johnson1@example.com" xr:uid="{D5D75DC1-E84C-A642-A041-2C64364D7F71}"/>
-    <hyperlink ref="C2:C52" r:id="rId2" display="b.johnson1@example.com" xr:uid="{131ADCCB-BF8C-D146-9103-B095F3FA660A}"/>
+    <hyperlink ref="C2" r:id="rId1" display="b.johnson1@example.com" xr:uid="{D5D75DC1-E84C-A642-A041-2C64364D7F71}"/>
+    <hyperlink ref="C3:C53" r:id="rId2" display="b.johnson1@example.com" xr:uid="{131ADCCB-BF8C-D146-9103-B095F3FA660A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>